<commit_message>
Refatoração para deixar mais simples a implementação da leitura de arquivo xlsx, e troca de biblioteca de ClosedXML para MiniExcel.
</commit_message>
<xml_diff>
--- a/arquivos/REM22062023_BIKE.xlsx
+++ b/arquivos/REM22062023_BIKE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Allan\Programacao\Projetos\.NET\GIT-Pessoal\FileManagement\arquivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\GIT - Pessoal\File Management\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF5C372-FB0B-4C7C-A00B-5D2D56503848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,6 +36,12 @@
     <t>Bike</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
     <t>Product</t>
   </si>
   <si>
@@ -42,18 +49,12 @@
   </si>
   <si>
     <t>IsNew</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -364,11 +365,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -378,13 +379,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -395,7 +396,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -406,7 +407,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -417,7 +418,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -428,7 +429,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -439,7 +440,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -450,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -461,7 +462,7 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -472,7 +473,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -483,7 +484,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -494,7 +495,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -505,7 +506,7 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -516,7 +517,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -527,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -538,7 +539,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -549,7 +550,7 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -560,7 +561,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -571,7 +572,7 @@
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -582,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -593,7 +594,7 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -604,7 +605,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -615,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -626,7 +627,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>